<commit_message>
approach5 corrected and new summary generated
</commit_message>
<xml_diff>
--- a/notebooks_rotten_tomatoes/test_cases_rotten_tomatoes_adson/summary.xlsx
+++ b/notebooks_rotten_tomatoes/test_cases_rotten_tomatoes_adson/summary.xlsx
@@ -1,19 +1,19 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<workbook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <workbookPr/>
   <workbookProtection/>
   <bookViews>
     <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" tabRatio="600" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
   </bookViews>
   <sheets>
-    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="approach1.xlsx" sheetId="1" state="visible" r:id="rId1"/>
-    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="approach2.xlsx" sheetId="2" state="visible" r:id="rId2"/>
-    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="approach3.xlsx" sheetId="3" state="visible" r:id="rId3"/>
-    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="approach4.xlsx" sheetId="4" state="visible" r:id="rId4"/>
-    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="approach5.xlsx" sheetId="5" state="visible" r:id="rId5"/>
-    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="random.xlsx" sheetId="6" state="visible" r:id="rId6"/>
-    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="general_summary" sheetId="7" state="visible" r:id="rId7"/>
+    <sheet name="approach1.xlsx" sheetId="1" state="visible" r:id="rId1"/>
+    <sheet name="approach2.xlsx" sheetId="2" state="visible" r:id="rId2"/>
+    <sheet name="approach3.xlsx" sheetId="3" state="visible" r:id="rId3"/>
+    <sheet name="approach4.xlsx" sheetId="4" state="visible" r:id="rId4"/>
+    <sheet name="approach5.xlsx" sheetId="5" state="visible" r:id="rId5"/>
+    <sheet name="random.xlsx" sheetId="6" state="visible" r:id="rId6"/>
+    <sheet name="general_summary" sheetId="7" state="visible" r:id="rId7"/>
   </sheets>
   <definedNames/>
   <calcPr calcId="124519" fullCalcOnLoad="1"/>
@@ -2727,7 +2727,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:N25"/>
+  <dimension ref="A1:N26"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -3454,17 +3454,17 @@
     <row r="16">
       <c r="A16" t="inlineStr">
         <is>
-          <t>template16</t>
+          <t>template15</t>
         </is>
       </c>
       <c r="B16" t="n">
-        <v>2</v>
+        <v>14</v>
       </c>
       <c r="C16" t="n">
-        <v>2</v>
+        <v>9</v>
       </c>
       <c r="D16" t="n">
-        <v>0</v>
+        <v>5</v>
       </c>
       <c r="E16" t="n">
         <v>0</v>
@@ -3473,10 +3473,10 @@
         <v>0</v>
       </c>
       <c r="G16" t="n">
-        <v>2</v>
+        <v>9</v>
       </c>
       <c r="H16" t="n">
-        <v>0</v>
+        <v>5</v>
       </c>
       <c r="I16" t="n">
         <v>0</v>
@@ -3500,14 +3500,14 @@
     <row r="17">
       <c r="A17" t="inlineStr">
         <is>
-          <t>template17</t>
+          <t>template16</t>
         </is>
       </c>
       <c r="B17" t="n">
-        <v>28</v>
+        <v>2</v>
       </c>
       <c r="C17" t="n">
-        <v>28</v>
+        <v>2</v>
       </c>
       <c r="D17" t="n">
         <v>0</v>
@@ -3519,7 +3519,7 @@
         <v>0</v>
       </c>
       <c r="G17" t="n">
-        <v>28</v>
+        <v>2</v>
       </c>
       <c r="H17" t="n">
         <v>0</v>
@@ -3546,35 +3546,35 @@
     <row r="18">
       <c r="A18" t="inlineStr">
         <is>
-          <t>template18</t>
+          <t>template17</t>
         </is>
       </c>
       <c r="B18" t="n">
-        <v>38</v>
+        <v>28</v>
       </c>
       <c r="C18" t="n">
-        <v>8</v>
+        <v>28</v>
       </c>
       <c r="D18" t="n">
-        <v>30</v>
+        <v>0</v>
       </c>
       <c r="E18" t="n">
-        <v>4</v>
+        <v>0</v>
       </c>
       <c r="F18" t="n">
-        <v>17</v>
+        <v>0</v>
       </c>
       <c r="G18" t="n">
-        <v>4</v>
+        <v>28</v>
       </c>
       <c r="H18" t="n">
-        <v>13</v>
+        <v>0</v>
       </c>
       <c r="I18" t="n">
         <v>0</v>
       </c>
       <c r="J18" t="n">
-        <v>4</v>
+        <v>0</v>
       </c>
       <c r="K18" t="n">
         <v>0</v>
@@ -3583,7 +3583,7 @@
         <v>0</v>
       </c>
       <c r="M18" t="n">
-        <v>17</v>
+        <v>0</v>
       </c>
       <c r="N18" t="n">
         <v>0</v>
@@ -3592,35 +3592,35 @@
     <row r="19">
       <c r="A19" t="inlineStr">
         <is>
-          <t>template19</t>
+          <t>template18</t>
         </is>
       </c>
       <c r="B19" t="n">
-        <v>28</v>
+        <v>38</v>
       </c>
       <c r="C19" t="n">
-        <v>28</v>
+        <v>8</v>
       </c>
       <c r="D19" t="n">
-        <v>0</v>
+        <v>30</v>
       </c>
       <c r="E19" t="n">
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="F19" t="n">
-        <v>0</v>
+        <v>17</v>
       </c>
       <c r="G19" t="n">
-        <v>28</v>
+        <v>4</v>
       </c>
       <c r="H19" t="n">
-        <v>0</v>
+        <v>13</v>
       </c>
       <c r="I19" t="n">
         <v>0</v>
       </c>
       <c r="J19" t="n">
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="K19" t="n">
         <v>0</v>
@@ -3629,7 +3629,7 @@
         <v>0</v>
       </c>
       <c r="M19" t="n">
-        <v>0</v>
+        <v>17</v>
       </c>
       <c r="N19" t="n">
         <v>0</v>
@@ -3638,14 +3638,14 @@
     <row r="20">
       <c r="A20" t="inlineStr">
         <is>
-          <t>template20</t>
+          <t>template19</t>
         </is>
       </c>
       <c r="B20" t="n">
-        <v>2</v>
+        <v>28</v>
       </c>
       <c r="C20" t="n">
-        <v>2</v>
+        <v>28</v>
       </c>
       <c r="D20" t="n">
         <v>0</v>
@@ -3657,7 +3657,7 @@
         <v>0</v>
       </c>
       <c r="G20" t="n">
-        <v>2</v>
+        <v>28</v>
       </c>
       <c r="H20" t="n">
         <v>0</v>
@@ -3684,35 +3684,35 @@
     <row r="21">
       <c r="A21" t="inlineStr">
         <is>
-          <t>template21</t>
+          <t>template20</t>
         </is>
       </c>
       <c r="B21" t="n">
-        <v>6</v>
+        <v>2</v>
       </c>
       <c r="C21" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="D21" t="n">
-        <v>5</v>
+        <v>0</v>
       </c>
       <c r="E21" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F21" t="n">
-        <v>4</v>
+        <v>0</v>
       </c>
       <c r="G21" t="n">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="H21" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I21" t="n">
         <v>0</v>
       </c>
       <c r="J21" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="K21" t="n">
         <v>0</v>
@@ -3721,7 +3721,7 @@
         <v>0</v>
       </c>
       <c r="M21" t="n">
-        <v>4</v>
+        <v>0</v>
       </c>
       <c r="N21" t="n">
         <v>0</v>
@@ -3730,35 +3730,35 @@
     <row r="22">
       <c r="A22" t="inlineStr">
         <is>
-          <t>template22</t>
+          <t>template21</t>
         </is>
       </c>
       <c r="B22" t="n">
-        <v>2</v>
+        <v>6</v>
       </c>
       <c r="C22" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="D22" t="n">
-        <v>0</v>
+        <v>5</v>
       </c>
       <c r="E22" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F22" t="n">
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="G22" t="n">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="H22" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I22" t="n">
         <v>0</v>
       </c>
       <c r="J22" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="K22" t="n">
         <v>0</v>
@@ -3767,7 +3767,7 @@
         <v>0</v>
       </c>
       <c r="M22" t="n">
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="N22" t="n">
         <v>0</v>
@@ -3776,29 +3776,29 @@
     <row r="23">
       <c r="A23" t="inlineStr">
         <is>
-          <t>template23</t>
+          <t>template22</t>
         </is>
       </c>
       <c r="B23" t="n">
-        <v>10</v>
+        <v>2</v>
       </c>
       <c r="C23" t="n">
-        <v>5</v>
+        <v>2</v>
       </c>
       <c r="D23" t="n">
-        <v>5</v>
+        <v>0</v>
       </c>
       <c r="E23" t="n">
         <v>0</v>
       </c>
       <c r="F23" t="n">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="G23" t="n">
-        <v>5</v>
+        <v>2</v>
       </c>
       <c r="H23" t="n">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="I23" t="n">
         <v>0</v>
@@ -3813,7 +3813,7 @@
         <v>0</v>
       </c>
       <c r="M23" t="n">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="N23" t="n">
         <v>0</v>
@@ -3822,29 +3822,29 @@
     <row r="24">
       <c r="A24" t="inlineStr">
         <is>
-          <t>template24</t>
+          <t>template23</t>
         </is>
       </c>
       <c r="B24" t="n">
-        <v>28</v>
+        <v>10</v>
       </c>
       <c r="C24" t="n">
-        <v>8</v>
+        <v>5</v>
       </c>
       <c r="D24" t="n">
-        <v>20</v>
+        <v>5</v>
       </c>
       <c r="E24" t="n">
-        <v>8</v>
+        <v>0</v>
       </c>
       <c r="F24" t="n">
-        <v>20</v>
+        <v>2</v>
       </c>
       <c r="G24" t="n">
-        <v>0</v>
+        <v>5</v>
       </c>
       <c r="H24" t="n">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="I24" t="n">
         <v>0</v>
@@ -3853,61 +3853,107 @@
         <v>0</v>
       </c>
       <c r="K24" t="n">
-        <v>8</v>
+        <v>0</v>
       </c>
       <c r="L24" t="n">
         <v>0</v>
       </c>
       <c r="M24" t="n">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="N24" t="n">
-        <v>20</v>
+        <v>0</v>
       </c>
     </row>
     <row r="25">
       <c r="A25" t="inlineStr">
         <is>
+          <t>template24</t>
+        </is>
+      </c>
+      <c r="B25" t="n">
+        <v>28</v>
+      </c>
+      <c r="C25" t="n">
+        <v>8</v>
+      </c>
+      <c r="D25" t="n">
+        <v>20</v>
+      </c>
+      <c r="E25" t="n">
+        <v>8</v>
+      </c>
+      <c r="F25" t="n">
+        <v>20</v>
+      </c>
+      <c r="G25" t="n">
+        <v>0</v>
+      </c>
+      <c r="H25" t="n">
+        <v>0</v>
+      </c>
+      <c r="I25" t="n">
+        <v>0</v>
+      </c>
+      <c r="J25" t="n">
+        <v>0</v>
+      </c>
+      <c r="K25" t="n">
+        <v>8</v>
+      </c>
+      <c r="L25" t="n">
+        <v>0</v>
+      </c>
+      <c r="M25" t="n">
+        <v>0</v>
+      </c>
+      <c r="N25" t="n">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="26">
+      <c r="A26" t="inlineStr">
+        <is>
           <t>template25</t>
         </is>
       </c>
-      <c r="B25" t="n">
+      <c r="B26" t="n">
         <v>19</v>
       </c>
-      <c r="C25" t="n">
+      <c r="C26" t="n">
         <v>16</v>
       </c>
-      <c r="D25" t="n">
-        <v>3</v>
-      </c>
-      <c r="E25" t="n">
-        <v>2</v>
-      </c>
-      <c r="F25" t="n">
-        <v>3</v>
-      </c>
-      <c r="G25" t="n">
+      <c r="D26" t="n">
+        <v>3</v>
+      </c>
+      <c r="E26" t="n">
+        <v>2</v>
+      </c>
+      <c r="F26" t="n">
+        <v>3</v>
+      </c>
+      <c r="G26" t="n">
         <v>14</v>
       </c>
-      <c r="H25" t="n">
-        <v>0</v>
-      </c>
-      <c r="I25" t="n">
-        <v>0</v>
-      </c>
-      <c r="J25" t="n">
-        <v>2</v>
-      </c>
-      <c r="K25" t="n">
-        <v>0</v>
-      </c>
-      <c r="L25" t="n">
-        <v>0</v>
-      </c>
-      <c r="M25" t="n">
-        <v>3</v>
-      </c>
-      <c r="N25" t="n">
+      <c r="H26" t="n">
+        <v>0</v>
+      </c>
+      <c r="I26" t="n">
+        <v>0</v>
+      </c>
+      <c r="J26" t="n">
+        <v>2</v>
+      </c>
+      <c r="K26" t="n">
+        <v>0</v>
+      </c>
+      <c r="L26" t="n">
+        <v>0</v>
+      </c>
+      <c r="M26" t="n">
+        <v>3</v>
+      </c>
+      <c r="N26" t="n">
         <v>0</v>
       </c>
     </row>
@@ -5262,22 +5308,22 @@
         </is>
       </c>
       <c r="B6" t="n">
-        <v>372</v>
+        <v>386</v>
       </c>
       <c r="C6" t="n">
-        <v>221</v>
+        <v>230</v>
       </c>
       <c r="D6" t="inlineStr">
         <is>
-          <t>59.4</t>
+          <t>59.6</t>
         </is>
       </c>
       <c r="E6" t="n">
-        <v>151</v>
+        <v>156</v>
       </c>
       <c r="F6" t="inlineStr">
         <is>
-          <t>40.6</t>
+          <t>40.4</t>
         </is>
       </c>
       <c r="G6" t="n">
@@ -5285,7 +5331,7 @@
       </c>
       <c r="H6" t="inlineStr">
         <is>
-          <t>5.1</t>
+          <t>4.9</t>
         </is>
       </c>
       <c r="I6" t="n">
@@ -5293,23 +5339,23 @@
       </c>
       <c r="J6" t="inlineStr">
         <is>
-          <t>16.9</t>
+          <t>16.3</t>
         </is>
       </c>
       <c r="K6" t="n">
-        <v>202</v>
+        <v>211</v>
       </c>
       <c r="L6" t="inlineStr">
         <is>
-          <t>54.3</t>
+          <t>54.7</t>
         </is>
       </c>
       <c r="M6" t="n">
-        <v>88</v>
+        <v>93</v>
       </c>
       <c r="N6" t="inlineStr">
         <is>
-          <t>23.7</t>
+          <t>24.1</t>
         </is>
       </c>
       <c r="O6" t="n">

</xml_diff>

<commit_message>
some charts to a better comparation
</commit_message>
<xml_diff>
--- a/notebooks_rotten_tomatoes/test_cases_rotten_tomatoes_adson/summary.xlsx
+++ b/notebooks_rotten_tomatoes/test_cases_rotten_tomatoes_adson/summary.xlsx
@@ -492,7 +492,7 @@
       </c>
       <c r="K1" s="1" t="inlineStr">
         <is>
-          <t>FN_NO</t>
+          <t>FN_TE</t>
         </is>
       </c>
       <c r="L1" s="1" t="inlineStr">
@@ -629,7 +629,7 @@
       </c>
       <c r="K1" s="1" t="inlineStr">
         <is>
-          <t>FN_NO</t>
+          <t>FN_TE</t>
         </is>
       </c>
       <c r="L1" s="1" t="inlineStr">
@@ -812,7 +812,7 @@
       </c>
       <c r="K1" s="1" t="inlineStr">
         <is>
-          <t>FN_NO</t>
+          <t>FN_TE</t>
         </is>
       </c>
       <c r="L1" s="1" t="inlineStr">
@@ -1823,7 +1823,7 @@
       </c>
       <c r="K1" s="1" t="inlineStr">
         <is>
-          <t>FN_NO</t>
+          <t>FN_TE</t>
         </is>
       </c>
       <c r="L1" s="1" t="inlineStr">
@@ -2788,7 +2788,7 @@
       </c>
       <c r="K1" s="1" t="inlineStr">
         <is>
-          <t>FN_NO</t>
+          <t>FN_TE</t>
         </is>
       </c>
       <c r="L1" s="1" t="inlineStr">
@@ -4029,7 +4029,7 @@
       </c>
       <c r="K1" s="1" t="inlineStr">
         <is>
-          <t>FN_NO</t>
+          <t>FN_TE</t>
         </is>
       </c>
       <c r="L1" s="1" t="inlineStr">
@@ -4978,7 +4978,7 @@
       </c>
       <c r="Q1" s="1" t="inlineStr">
         <is>
-          <t>FN_NO</t>
+          <t>FN_TE</t>
         </is>
       </c>
       <c r="R1" s="1" t="inlineStr">

</xml_diff>

<commit_message>
correct summary error; create comparing notebook
</commit_message>
<xml_diff>
--- a/notebooks_rotten_tomatoes/test_cases_rotten_tomatoes_adson/summary.xlsx
+++ b/notebooks_rotten_tomatoes/test_cases_rotten_tomatoes_adson/summary.xlsx
@@ -1,19 +1,19 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <workbookPr/>
   <workbookProtection/>
   <bookViews>
     <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" tabRatio="600" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
   </bookViews>
   <sheets>
-    <sheet name="approach1.xlsx" sheetId="1" state="visible" r:id="rId1"/>
-    <sheet name="approach2.xlsx" sheetId="2" state="visible" r:id="rId2"/>
-    <sheet name="approach3.xlsx" sheetId="3" state="visible" r:id="rId3"/>
-    <sheet name="approach4.xlsx" sheetId="4" state="visible" r:id="rId4"/>
-    <sheet name="approach5.xlsx" sheetId="5" state="visible" r:id="rId5"/>
-    <sheet name="random.xlsx" sheetId="6" state="visible" r:id="rId6"/>
-    <sheet name="general_summary" sheetId="7" state="visible" r:id="rId7"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="approach1.xlsx" sheetId="1" state="visible" r:id="rId1"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="approach2.xlsx" sheetId="2" state="visible" r:id="rId2"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="approach3.xlsx" sheetId="3" state="visible" r:id="rId3"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="approach4.xlsx" sheetId="4" state="visible" r:id="rId4"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="approach5.xlsx" sheetId="5" state="visible" r:id="rId5"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="random.xlsx" sheetId="6" state="visible" r:id="rId6"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="general_summary" sheetId="7" state="visible" r:id="rId7"/>
   </sheets>
   <definedNames/>
   <calcPr calcId="124519" fullCalcOnLoad="1"/>
@@ -5027,7 +5027,7 @@
       </c>
       <c r="H2" t="inlineStr">
         <is>
-          <t>50.0</t>
+          <t>100.0</t>
         </is>
       </c>
       <c r="I2" t="n">
@@ -5035,7 +5035,7 @@
       </c>
       <c r="J2" t="inlineStr">
         <is>
-          <t>50.0</t>
+          <t>100.0</t>
         </is>
       </c>
       <c r="K2" t="n">
@@ -5103,7 +5103,7 @@
       </c>
       <c r="H3" t="inlineStr">
         <is>
-          <t>33.3</t>
+          <t>40.0</t>
         </is>
       </c>
       <c r="I3" t="n">
@@ -5111,7 +5111,7 @@
       </c>
       <c r="J3" t="inlineStr">
         <is>
-          <t>16.7</t>
+          <t>100.0</t>
         </is>
       </c>
       <c r="K3" t="n">
@@ -5119,7 +5119,7 @@
       </c>
       <c r="L3" t="inlineStr">
         <is>
-          <t>50.0</t>
+          <t>60.0</t>
         </is>
       </c>
       <c r="M3" t="n">
@@ -5179,7 +5179,7 @@
       </c>
       <c r="H4" t="inlineStr">
         <is>
-          <t>6.8</t>
+          <t>9.8</t>
         </is>
       </c>
       <c r="I4" t="n">
@@ -5187,7 +5187,7 @@
       </c>
       <c r="J4" t="inlineStr">
         <is>
-          <t>19.5</t>
+          <t>63.8</t>
         </is>
       </c>
       <c r="K4" t="n">
@@ -5195,7 +5195,7 @@
       </c>
       <c r="L4" t="inlineStr">
         <is>
-          <t>61.7</t>
+          <t>88.8</t>
         </is>
       </c>
       <c r="M4" t="n">
@@ -5203,7 +5203,7 @@
       </c>
       <c r="N4" t="inlineStr">
         <is>
-          <t>12.0</t>
+          <t>39.4</t>
         </is>
       </c>
       <c r="O4" t="n">
@@ -5255,7 +5255,7 @@
       </c>
       <c r="H5" t="inlineStr">
         <is>
-          <t>8.8</t>
+          <t>12.6</t>
         </is>
       </c>
       <c r="I5" t="n">
@@ -5263,7 +5263,7 @@
       </c>
       <c r="J5" t="inlineStr">
         <is>
-          <t>15.6</t>
+          <t>52.9</t>
         </is>
       </c>
       <c r="K5" t="n">
@@ -5271,7 +5271,7 @@
       </c>
       <c r="L5" t="inlineStr">
         <is>
-          <t>61.6</t>
+          <t>87.4</t>
         </is>
       </c>
       <c r="M5" t="n">
@@ -5279,7 +5279,7 @@
       </c>
       <c r="N5" t="inlineStr">
         <is>
-          <t>13.9</t>
+          <t>47.1</t>
         </is>
       </c>
       <c r="O5" t="n">
@@ -5331,7 +5331,7 @@
       </c>
       <c r="H6" t="inlineStr">
         <is>
-          <t>4.9</t>
+          <t>8.3</t>
         </is>
       </c>
       <c r="I6" t="n">
@@ -5339,7 +5339,7 @@
       </c>
       <c r="J6" t="inlineStr">
         <is>
-          <t>16.3</t>
+          <t>40.4</t>
         </is>
       </c>
       <c r="K6" t="n">
@@ -5347,7 +5347,7 @@
       </c>
       <c r="L6" t="inlineStr">
         <is>
-          <t>54.7</t>
+          <t>91.7</t>
         </is>
       </c>
       <c r="M6" t="n">
@@ -5355,7 +5355,7 @@
       </c>
       <c r="N6" t="inlineStr">
         <is>
-          <t>24.1</t>
+          <t>59.6</t>
         </is>
       </c>
       <c r="O6" t="n">
@@ -5407,7 +5407,7 @@
       </c>
       <c r="H7" t="inlineStr">
         <is>
-          <t>35.4</t>
+          <t>44.5</t>
         </is>
       </c>
       <c r="I7" t="n">
@@ -5415,7 +5415,7 @@
       </c>
       <c r="J7" t="inlineStr">
         <is>
-          <t>14.4</t>
+          <t>70.2</t>
         </is>
       </c>
       <c r="K7" t="n">
@@ -5423,7 +5423,7 @@
       </c>
       <c r="L7" t="inlineStr">
         <is>
-          <t>44.1</t>
+          <t>55.5</t>
         </is>
       </c>
       <c r="M7" t="n">
@@ -5431,7 +5431,7 @@
       </c>
       <c r="N7" t="inlineStr">
         <is>
-          <t>6.1</t>
+          <t>29.8</t>
         </is>
       </c>
       <c r="O7" t="n">

</xml_diff>